<commit_message>
TTC Unfiltered eveals for doc
</commit_message>
<xml_diff>
--- a/evaluations/MAT_FLANN_SEL_KNN_Filtered.xlsx
+++ b/evaluations/MAT_FLANN_SEL_KNN_Filtered.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsumaka\Desktop\3D_Object_Tracking\evaluations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2794FCF6-CB37-411B-8513-279FAA687123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E37DD4-0164-4280-87F0-58AA355EEE6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="285" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAT_FLANN_SEL_KNN" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3450,14 +3450,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -3785,7 +3785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>